<commit_message>
Update : MAS Report templates formatting
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx-templates/mas-report-1a.xlsx
+++ b/src/main/resources/xlsx-templates/mas-report-1a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProject\dtc-settlement-engine\src\main\resources\xlsx-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552D536F-1485-40F3-9DA6-4FEEBED2EDAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97044D19-B622-4B9E-954C-828EBD6C004A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36960" yWindow="555" windowWidth="20145" windowHeight="13725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1A Summary" sheetId="5" r:id="rId1"/>
@@ -108,6 +108,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -553,13 +556,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -577,6 +574,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -607,29 +628,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -848,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC7A168-8554-4268-ACD7-9F07E022F1C7}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -858,32 +861,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" spans="1:3" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -900,28 +903,20 @@
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8">
-        <v>0</v>
-      </c>
-      <c r="C6" s="9">
-        <v>0</v>
-      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="10">
-        <v>0</v>
-      </c>
-      <c r="C7" s="11">
-        <v>0</v>
-      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -938,117 +933,101 @@
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8">
-        <v>0</v>
-      </c>
-      <c r="C10" s="9">
-        <v>0</v>
-      </c>
+      <c r="B10" s="32"/>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="10">
-        <v>0</v>
-      </c>
-      <c r="C11" s="11">
-        <v>0</v>
-      </c>
+      <c r="B11" s="33"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="27"/>
+      <c r="C13" s="17"/>
     </row>
     <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="16">
-        <v>0</v>
-      </c>
-      <c r="C14" s="17"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
     </row>
     <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="16">
-        <v>0</v>
-      </c>
-      <c r="C15" s="17"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
     </row>
     <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="16">
-        <v>0</v>
-      </c>
-      <c r="C16" s="17"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
     </row>
     <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="16">
-        <v>0</v>
-      </c>
-      <c r="C17" s="17"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
     </row>
     <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="16">
-        <v>0</v>
-      </c>
-      <c r="C18" s="17"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="23"/>
     </row>
     <row r="19" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="28">
-        <v>0</v>
-      </c>
-      <c r="C19" s="29"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
     </row>
     <row r="20" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
     </row>
     <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="27"/>
+      <c r="C21" s="17"/>
     </row>
     <row r="22" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
-      <c r="B22" s="30">
-        <v>0</v>
-      </c>
-      <c r="C22" s="31"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
+      <c r="A23" s="12"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
+      <c r="A24" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
@@ -1057,12 +1036,6 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>